<commit_message>
able to scrape and extract data
</commit_message>
<xml_diff>
--- a/Zillow_Realtors.xlsx
+++ b/Zillow_Realtors.xlsx
@@ -1,60 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2a3a8cdee718e8c2/Documents/coding/Python/scrape_zil_rel/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_E8A970ACDE721CBEE11CBCB743245E3F848BF2BC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD4123CE-451B-4245-87F2-FBEC23E8D9E9}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Realtors on Zil" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Realtors on Zil" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Kris Lindahl</t>
-  </si>
-  <si>
-    <t>/profile/KrisLindahl/</t>
-  </si>
-  <si>
-    <t>Michael Gross</t>
-  </si>
-  <si>
-    <t>/profile/MichaelGross/</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -69,43 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -393,43 +420,419 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AE3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B1" s="1">
+    <row r="1">
+      <c r="B1" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1" t="n">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+    <row r="2">
+      <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Chris and Natalie and the Story Team</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Tanja Blue</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Aline Gale</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>RE/MAX Connections Teri Skiles</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>David Dail</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Susan Miller</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Eric Burnett</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Tyler LaVoie</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Jason Brown</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Angela Foisy</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Chris and Natalie and the Story Team</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Tanja Blue</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Aline Gale</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>RE/MAX Connections Teri Skiles</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>David Dail</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Susan Miller</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Eric Burnett</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Tyler LaVoie</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Jason Brown</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>Angela Foisy</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>Kathi Nygaard</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>Kathryn Church</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>Brian Howard</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>Danny Bradley</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>Jordan Clemans</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>Leah Clark</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>Mike Church</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>Sam Christensen</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>Traci Hacker</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>Jennifer O'Brien</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>/profile/sremoscow/</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>/profile/Tanja-Blue/</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>/profile/Aline-Gale/</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>/profile/Teri-Skiles/</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>/profile/davepdail/</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>/profile/Mary-Susan-Miller/</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>/profile/ericburnetthomes/</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>/profile/tylerlavoie1/</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>/profile/JasonBrown-Realtor/</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>/profile/AngelaFoisy/</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>/profile/sremoscow/</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>/profile/Tanja-Blue/</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>/profile/Aline-Gale/</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>/profile/Teri-Skiles/</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>/profile/davepdail/</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>/profile/Mary-Susan-Miller/</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>/profile/ericburnetthomes/</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>/profile/tylerlavoie1/</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>/profile/JasonBrown-Realtor/</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>/profile/AngelaFoisy/</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>/profile/KathiLovesRealEstate/</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>/profile/kestrelrealty/</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>/profile/Brianhowardmoscow/</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>/profile/danny6241/</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>/profile/JordanClemans/</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>/profile/Leah-Clark-KW-Palous/</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>/profile/mikechurchkestrel/</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>/profile/Samchristensen208/</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>/profile/TraciHacker/</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>/profile/Jennifer-OBrien/</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>